<commit_message>
Fixed failing excel import tests.
git-svn-id: https://subversion.assembla.com/svn/treesdb/branches/ExcelImport@316 d913c9e1-59cf-094f-9d4b-ab1779aea92f
</commit_message>
<xml_diff>
--- a/TMD.UnitTests/Model/TMD.xlsx
+++ b/TMD.UnitTests/Model/TMD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14505" yWindow="-15" windowWidth="14310" windowHeight="14355" tabRatio="408" activeTab="3"/>
+    <workbookView xWindow="14505" yWindow="-15" windowWidth="14310" windowHeight="14355" tabRatio="408"/>
   </bookViews>
   <sheets>
     <sheet name="Sites" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Trees" sheetId="3" r:id="rId3"/>
     <sheet name="Trunks" sheetId="4" r:id="rId4"/>
     <sheet name="Internal" sheetId="5" state="hidden" r:id="rId5"/>
+    <sheet name="Photos" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Trees!$B$3:$B$100003</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4196" uniqueCount="3635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4197" uniqueCount="3636">
   <si>
     <t>Latitude</t>
   </si>
@@ -11053,6 +11054,9 @@
   </si>
   <si>
     <t>hello world</t>
+  </si>
+  <si>
+    <t>TODO: unit test this sheet</t>
   </si>
 </sst>
 </file>
@@ -12322,59 +12326,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
@@ -12482,6 +12433,59 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="969">
@@ -13908,7 +13912,7 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -13948,82 +13952,82 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="14" t="s">
         <v>3592</v>
       </c>
-      <c r="B2" s="38">
+      <c r="B2" s="15">
         <v>42.638353000000002</v>
       </c>
-      <c r="C2" s="38">
+      <c r="C2" s="15">
         <v>-72.936442999999997</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="16" t="s">
         <v>3596</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="19" t="s">
         <v>3597</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="14" t="s">
         <v>3593</v>
       </c>
-      <c r="B3" s="38">
+      <c r="B3" s="15">
         <v>42.278376999999999</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="15">
         <v>-73.307406999999998</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="16" t="s">
         <v>3596</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="19" t="s">
         <v>3598</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="14" t="s">
         <v>3594</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4" s="15">
         <v>42.469546000000001</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="15">
         <v>-72.931766999999994</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="16" t="s">
         <v>3596</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="F4" s="42" t="s">
+      <c r="F4" s="19" t="s">
         <v>3599</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="14" t="s">
         <v>3595</v>
       </c>
-      <c r="B5" s="38">
+      <c r="B5" s="15">
         <v>42.313014000000003</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="15">
         <v>-72.629553999999999</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="16" t="s">
         <v>3596</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="18"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0" insertHyperlinks="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
@@ -14106,205 +14110,205 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="20" t="s">
         <v>3592</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="21" t="s">
         <v>3600</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="22" t="s">
         <v>3607</v>
       </c>
-      <c r="F2" s="46">
+      <c r="F2" s="23">
         <v>42.643481999999999</v>
       </c>
-      <c r="G2" s="46">
+      <c r="G2" s="23">
         <v>-72.935085000000001</v>
       </c>
-      <c r="I2" s="47" t="s">
+      <c r="I2" s="24" t="s">
         <v>3535</v>
       </c>
-      <c r="J2" s="48" t="s">
+      <c r="J2" s="25" t="s">
         <v>3611</v>
       </c>
-      <c r="K2" s="50" t="s">
+      <c r="K2" s="27" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="20" t="s">
         <v>3592</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="21" t="s">
         <v>3601</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="22" t="s">
         <v>3607</v>
       </c>
-      <c r="F3" s="46">
+      <c r="F3" s="23">
         <v>42.549442999999997</v>
       </c>
-      <c r="G3" s="46">
+      <c r="G3" s="23">
         <v>-72.935023999999999</v>
       </c>
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="24" t="s">
         <v>3535</v>
       </c>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="25" t="s">
         <v>3611</v>
       </c>
-      <c r="K3" s="50" t="s">
+      <c r="K3" s="27" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="20" t="s">
         <v>3592</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="21" t="s">
         <v>3602</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="22" t="s">
         <v>3607</v>
       </c>
-      <c r="F4" s="46">
+      <c r="F4" s="23">
         <v>42.641773999999998</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="23">
         <v>-72.940648999999993</v>
       </c>
-      <c r="I4" s="47" t="s">
+      <c r="I4" s="24" t="s">
         <v>3535</v>
       </c>
-      <c r="J4" s="48" t="s">
+      <c r="J4" s="25" t="s">
         <v>3611</v>
       </c>
-      <c r="K4" s="50" t="s">
+      <c r="K4" s="27" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="20" t="s">
         <v>3594</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="21" t="s">
         <v>3603</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="22" t="s">
         <v>3608</v>
       </c>
-      <c r="F5" s="46">
+      <c r="F5" s="23">
         <v>42.473897999999998</v>
       </c>
-      <c r="G5" s="46">
+      <c r="G5" s="23">
         <v>-72.927712</v>
       </c>
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="24" t="s">
         <v>3533</v>
       </c>
-      <c r="J5" s="48" t="s">
+      <c r="J5" s="25" t="s">
         <v>3612</v>
       </c>
-      <c r="K5" s="50" t="s">
+      <c r="K5" s="27" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="20" t="s">
         <v>3593</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="21" t="s">
         <v>3604</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="22" t="s">
         <v>3609</v>
       </c>
-      <c r="F6" s="46">
+      <c r="F6" s="23">
         <v>42.275672999999998</v>
       </c>
-      <c r="G6" s="46">
+      <c r="G6" s="23">
         <v>-73.30753</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="24" t="s">
         <v>3533</v>
       </c>
-      <c r="J6" s="48" t="s">
+      <c r="J6" s="25" t="s">
         <v>3613</v>
       </c>
-      <c r="K6" s="50" t="s">
+      <c r="K6" s="27" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="20" t="s">
         <v>3595</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="21" t="s">
         <v>3605</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="22" t="s">
         <v>3610</v>
       </c>
-      <c r="F7" s="46">
+      <c r="F7" s="23">
         <v>42.313014000000003</v>
       </c>
-      <c r="G7" s="46">
+      <c r="G7" s="23">
         <v>-72.629553999999999</v>
       </c>
-      <c r="I7" s="47" t="s">
+      <c r="I7" s="24" t="s">
         <v>3533</v>
       </c>
-      <c r="J7" s="48" t="s">
+      <c r="J7" s="25" t="s">
         <v>3595</v>
       </c>
-      <c r="K7" s="50" t="s">
+      <c r="K7" s="27" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="20" t="s">
         <v>3592</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="21" t="s">
         <v>3606</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="22" t="s">
         <v>3607</v>
       </c>
-      <c r="F8" s="46">
+      <c r="F8" s="23">
         <v>42.650010999999999</v>
       </c>
-      <c r="G8" s="46">
+      <c r="G8" s="23">
         <v>-72.948763999999997</v>
       </c>
-      <c r="I8" s="47" t="s">
+      <c r="I8" s="24" t="s">
         <v>3535</v>
       </c>
-      <c r="J8" s="49" t="s">
+      <c r="J8" s="26" t="s">
         <v>3611</v>
       </c>
-      <c r="K8" s="50" t="s">
+      <c r="K8" s="27" t="s">
         <v>116</v>
       </c>
     </row>
@@ -14406,145 +14410,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="59" t="s">
         <v>3567</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="61" t="s">
         <v>3566</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="63" t="s">
         <v>3525</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="64" t="s">
         <v>3526</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="65" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="66" t="s">
         <v>156</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="67" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="66" t="s">
         <v>3585</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="70" t="s">
         <v>3572</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="66" t="s">
         <v>3569</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="71" t="s">
         <v>3523</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="71" t="s">
         <v>3524</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="67" t="s">
         <v>167</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="67" t="s">
         <v>154</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="67" t="s">
         <v>134</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="67" t="s">
         <v>140</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="S1" s="72" t="s">
         <v>3543</v>
       </c>
-      <c r="T1" s="31" t="s">
+      <c r="T1" s="68" t="s">
         <v>141</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="U1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="V1" s="17" t="s">
+      <c r="V1" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="W1" s="65" t="s">
         <v>3582</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="X1" s="67" t="s">
         <v>155</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Y1" s="66" t="s">
         <v>3588</v>
       </c>
-      <c r="Z1" s="23" t="s">
+      <c r="Z1" s="57" t="s">
         <v>119</v>
       </c>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="23"/>
-      <c r="AF1" s="23"/>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="23" t="s">
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="58"/>
+      <c r="AI1" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="AJ1" s="23"/>
-      <c r="AK1" s="24"/>
-      <c r="AL1" s="23" t="s">
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="58"/>
+      <c r="AL1" s="57" t="s">
         <v>3589</v>
       </c>
-      <c r="AM1" s="23"/>
-      <c r="AN1" s="23"/>
-      <c r="AO1" s="23"/>
-      <c r="AP1" s="23"/>
-      <c r="AQ1" s="23"/>
-      <c r="AR1" s="23"/>
-      <c r="AS1" s="24"/>
-      <c r="AT1" s="22" t="s">
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="58"/>
+      <c r="AT1" s="56" t="s">
         <v>3590</v>
       </c>
-      <c r="AU1" s="23"/>
-      <c r="AV1" s="23"/>
-      <c r="AW1" s="23"/>
-      <c r="AX1" s="22" t="s">
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
+      <c r="AW1" s="57"/>
+      <c r="AX1" s="56" t="s">
         <v>3591</v>
       </c>
-      <c r="AY1" s="23"/>
-      <c r="AZ1" s="24"/>
+      <c r="AY1" s="57"/>
+      <c r="AZ1" s="58"/>
     </row>
     <row r="2" spans="1:52" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="15"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="72"/>
+      <c r="T2" s="69"/>
+      <c r="U2" s="67"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="65"/>
+      <c r="X2" s="67"/>
+      <c r="Y2" s="66"/>
       <c r="Z2" s="4" t="s">
         <v>124</v>
       </c>
@@ -14628,716 +14632,716 @@
       </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="28" t="s">
         <v>3600</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="29" t="s">
         <v>3614</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="30" t="s">
         <v>3621</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="30" t="s">
         <v>1342</v>
       </c>
-      <c r="E3" s="54">
+      <c r="E3" s="31">
         <v>172.5</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="G3" s="64">
+      <c r="G3" s="41">
         <v>10.6</v>
       </c>
-      <c r="H3" s="65"/>
-      <c r="I3" s="73">
+      <c r="H3" s="42"/>
+      <c r="I3" s="50">
         <v>41614</v>
       </c>
-      <c r="J3" s="76" t="s">
+      <c r="J3" s="53" t="s">
         <v>3596</v>
       </c>
-      <c r="K3" s="76" t="s">
+      <c r="K3" s="53" t="s">
         <v>3631</v>
       </c>
-      <c r="L3" s="76" t="s">
+      <c r="L3" s="53" t="s">
         <v>3632</v>
       </c>
-      <c r="M3" s="69" t="s">
+      <c r="M3" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="O3" s="70" t="s">
+      <c r="O3" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="P3" s="70" t="s">
+      <c r="P3" s="47" t="s">
         <v>3629</v>
       </c>
-      <c r="Q3" s="70" t="s">
+      <c r="Q3" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="R3" s="70">
+      <c r="R3" s="47">
         <v>155</v>
       </c>
-      <c r="S3" s="70" t="s">
+      <c r="S3" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="T3" s="71" t="s">
+      <c r="T3" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="W3" s="74" t="s">
+      <c r="W3" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="X3" s="75">
+      <c r="X3" s="52">
         <v>800</v>
       </c>
-      <c r="Y3" s="72"/>
-      <c r="Z3" s="72" t="s">
+      <c r="Y3" s="49"/>
+      <c r="Z3" s="49" t="s">
         <v>3559</v>
       </c>
-      <c r="AA3" s="55" t="s">
+      <c r="AA3" s="32" t="s">
         <v>3559</v>
       </c>
-      <c r="AB3" s="57" t="s">
+      <c r="AB3" s="34" t="s">
         <v>3542</v>
       </c>
-      <c r="AC3" s="58"/>
-      <c r="AD3" s="58"/>
-      <c r="AE3" s="58"/>
-      <c r="AF3" s="58"/>
-      <c r="AG3" s="58"/>
-      <c r="AH3" s="61" t="s">
+      <c r="AC3" s="35"/>
+      <c r="AD3" s="35"/>
+      <c r="AE3" s="35"/>
+      <c r="AF3" s="35"/>
+      <c r="AG3" s="35"/>
+      <c r="AH3" s="38" t="s">
         <v>3624</v>
       </c>
-      <c r="AI3" s="63">
+      <c r="AI3" s="40">
         <v>4.5</v>
       </c>
-      <c r="AJ3" s="62"/>
-      <c r="AK3" s="62"/>
-      <c r="AL3" s="68">
+      <c r="AJ3" s="39"/>
+      <c r="AK3" s="39"/>
+      <c r="AL3" s="45">
         <v>48.5</v>
       </c>
-      <c r="AM3" s="68" t="s">
+      <c r="AM3" s="45" t="s">
         <v>3547</v>
       </c>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="28" t="s">
         <v>3604</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="29" t="s">
         <v>3615</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="30" t="s">
         <v>3621</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="D4" s="30" t="s">
         <v>1342</v>
       </c>
-      <c r="E4" s="54">
+      <c r="E4" s="31">
         <v>150</v>
       </c>
-      <c r="F4" s="54" t="s">
+      <c r="F4" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="G4" s="64">
+      <c r="G4" s="41">
         <v>12.4</v>
       </c>
-      <c r="H4" s="66">
+      <c r="H4" s="43">
         <v>52</v>
       </c>
-      <c r="I4" s="73">
+      <c r="I4" s="50">
         <v>41614</v>
       </c>
-      <c r="J4" s="76" t="s">
+      <c r="J4" s="53" t="s">
         <v>3596</v>
       </c>
-      <c r="K4" s="76" t="s">
+      <c r="K4" s="53" t="s">
         <v>3631</v>
       </c>
-      <c r="L4" s="76" t="s">
+      <c r="L4" s="53" t="s">
         <v>3632</v>
       </c>
-      <c r="M4" s="69" t="s">
+      <c r="M4" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="O4" s="70" t="s">
+      <c r="O4" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="P4" s="70" t="s">
+      <c r="P4" s="47" t="s">
         <v>3629</v>
       </c>
-      <c r="Q4" s="70" t="s">
+      <c r="Q4" s="47" t="s">
         <v>3530</v>
       </c>
-      <c r="R4" s="70">
+      <c r="R4" s="47">
         <v>190</v>
       </c>
-      <c r="S4" s="70" t="s">
+      <c r="S4" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="T4" s="71" t="s">
+      <c r="T4" s="48" t="s">
         <v>144</v>
       </c>
-      <c r="W4" s="72"/>
-      <c r="X4" s="72"/>
-      <c r="Y4" s="72"/>
-      <c r="Z4" s="72" t="s">
+      <c r="W4" s="49"/>
+      <c r="X4" s="49"/>
+      <c r="Y4" s="49"/>
+      <c r="Z4" s="49" t="s">
         <v>3558</v>
       </c>
-      <c r="AA4" s="55" t="s">
+      <c r="AA4" s="32" t="s">
         <v>3559</v>
       </c>
-      <c r="AB4" s="57" t="s">
+      <c r="AB4" s="34" t="s">
         <v>3540</v>
       </c>
-      <c r="AC4" s="59">
+      <c r="AC4" s="36">
         <v>192.89999999999998</v>
       </c>
-      <c r="AD4" s="59">
+      <c r="AD4" s="36">
         <v>45.2</v>
       </c>
-      <c r="AE4" s="59">
+      <c r="AE4" s="36">
         <v>136.5</v>
       </c>
-      <c r="AF4" s="59">
+      <c r="AF4" s="36">
         <v>-3.3</v>
       </c>
-      <c r="AG4" s="58"/>
-      <c r="AH4" s="60"/>
-      <c r="AI4" s="63">
+      <c r="AG4" s="35"/>
+      <c r="AH4" s="37"/>
+      <c r="AI4" s="40">
         <v>4.5</v>
       </c>
-      <c r="AJ4" s="63">
+      <c r="AJ4" s="40">
         <v>1</v>
       </c>
-      <c r="AK4" s="62"/>
-      <c r="AL4" s="68">
+      <c r="AK4" s="39"/>
+      <c r="AL4" s="45">
         <v>47</v>
       </c>
-      <c r="AM4" s="68" t="s">
+      <c r="AM4" s="45" t="s">
         <v>3548</v>
       </c>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="28" t="s">
         <v>3603</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="29" t="s">
         <v>3616</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="30" t="s">
         <v>3621</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="30" t="s">
         <v>1342</v>
       </c>
-      <c r="E5" s="54">
+      <c r="E5" s="31">
         <v>162.19999999999999</v>
       </c>
-      <c r="F5" s="54" t="s">
+      <c r="F5" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="G5" s="64">
+      <c r="G5" s="41">
         <v>10.199999999999999</v>
       </c>
-      <c r="H5" s="65"/>
-      <c r="I5" s="73">
+      <c r="H5" s="42"/>
+      <c r="I5" s="50">
         <v>41614</v>
       </c>
-      <c r="J5" s="76" t="s">
+      <c r="J5" s="53" t="s">
         <v>3596</v>
       </c>
-      <c r="K5" s="76" t="s">
+      <c r="K5" s="53" t="s">
         <v>3631</v>
       </c>
-      <c r="L5" s="76" t="s">
+      <c r="L5" s="53" t="s">
         <v>3632</v>
       </c>
-      <c r="M5" s="69" t="s">
+      <c r="M5" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="O5" s="70" t="s">
+      <c r="O5" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="P5" s="70" t="s">
+      <c r="P5" s="47" t="s">
         <v>3629</v>
       </c>
-      <c r="Q5" s="70" t="s">
+      <c r="Q5" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="R5" s="70">
+      <c r="R5" s="47">
         <v>130</v>
       </c>
-      <c r="S5" s="70" t="s">
+      <c r="S5" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="T5" s="71" t="s">
+      <c r="T5" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="Z5" s="55" t="s">
+      <c r="Z5" s="32" t="s">
         <v>3558</v>
       </c>
-      <c r="AA5" s="55" t="s">
+      <c r="AA5" s="32" t="s">
         <v>3562</v>
       </c>
-      <c r="AB5" s="57" t="s">
+      <c r="AB5" s="34" t="s">
         <v>3540</v>
       </c>
-      <c r="AC5" s="58"/>
-      <c r="AD5" s="58"/>
-      <c r="AE5" s="58"/>
-      <c r="AF5" s="58"/>
-      <c r="AG5" s="58"/>
-      <c r="AH5" s="61" t="s">
+      <c r="AC5" s="35"/>
+      <c r="AD5" s="35"/>
+      <c r="AE5" s="35"/>
+      <c r="AF5" s="35"/>
+      <c r="AG5" s="35"/>
+      <c r="AH5" s="38" t="s">
         <v>3625</v>
       </c>
-      <c r="AI5" s="63">
+      <c r="AI5" s="40">
         <v>4.5</v>
       </c>
-      <c r="AJ5" s="62"/>
-      <c r="AK5" s="62"/>
-      <c r="AL5" s="67"/>
-      <c r="AM5" s="67"/>
+      <c r="AJ5" s="39"/>
+      <c r="AK5" s="39"/>
+      <c r="AL5" s="44"/>
+      <c r="AM5" s="44"/>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="28" t="s">
         <v>3603</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="29" t="s">
         <v>3617</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="30" t="s">
         <v>3622</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="30" t="s">
         <v>1910</v>
       </c>
-      <c r="E6" s="54">
+      <c r="E6" s="31">
         <v>127</v>
       </c>
-      <c r="F6" s="54" t="s">
+      <c r="F6" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="G6" s="64">
+      <c r="G6" s="41">
         <v>9.1</v>
       </c>
-      <c r="H6" s="65"/>
-      <c r="I6" s="73">
+      <c r="H6" s="42"/>
+      <c r="I6" s="50">
         <v>41614</v>
       </c>
-      <c r="J6" s="76" t="s">
+      <c r="J6" s="53" t="s">
         <v>3596</v>
       </c>
-      <c r="K6" s="76" t="s">
+      <c r="K6" s="53" t="s">
         <v>3631</v>
       </c>
-      <c r="L6" s="76" t="s">
+      <c r="L6" s="53" t="s">
         <v>3632</v>
       </c>
-      <c r="M6" s="69" t="s">
+      <c r="M6" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="O6" s="70" t="s">
+      <c r="O6" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="P6" s="70" t="s">
+      <c r="P6" s="47" t="s">
         <v>3629</v>
       </c>
-      <c r="Q6" s="70" t="s">
+      <c r="Q6" s="47" t="s">
         <v>3530</v>
       </c>
-      <c r="R6" s="70">
+      <c r="R6" s="47">
         <v>175</v>
       </c>
-      <c r="S6" s="70" t="s">
+      <c r="S6" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="T6" s="71" t="s">
+      <c r="T6" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="Z6" s="55" t="s">
+      <c r="Z6" s="32" t="s">
         <v>3558</v>
       </c>
-      <c r="AA6" s="55" t="s">
+      <c r="AA6" s="32" t="s">
         <v>3559</v>
       </c>
-      <c r="AB6" s="57" t="s">
+      <c r="AB6" s="34" t="s">
         <v>3540</v>
       </c>
-      <c r="AC6" s="59">
+      <c r="AC6" s="36">
         <v>124.5</v>
       </c>
-      <c r="AD6" s="59">
+      <c r="AD6" s="36">
         <v>49.6</v>
       </c>
-      <c r="AE6" s="59">
+      <c r="AE6" s="36">
         <v>84</v>
       </c>
-      <c r="AF6" s="59">
+      <c r="AF6" s="36">
         <v>-22.5</v>
       </c>
-      <c r="AG6" s="58"/>
-      <c r="AH6" s="60"/>
-      <c r="AI6" s="63">
+      <c r="AG6" s="35"/>
+      <c r="AH6" s="37"/>
+      <c r="AI6" s="40">
         <v>4.5</v>
       </c>
-      <c r="AJ6" s="62"/>
-      <c r="AK6" s="62"/>
-      <c r="AL6" s="68">
+      <c r="AJ6" s="39"/>
+      <c r="AK6" s="39"/>
+      <c r="AL6" s="45">
         <v>39</v>
       </c>
-      <c r="AM6" s="68" t="s">
+      <c r="AM6" s="45" t="s">
         <v>3547</v>
       </c>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="28" t="s">
         <v>3601</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="29" t="s">
         <v>3618</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="30" t="s">
         <v>3621</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="D7" s="30" t="s">
         <v>1342</v>
       </c>
-      <c r="E7" s="54">
+      <c r="E7" s="31">
         <v>165</v>
       </c>
-      <c r="F7" s="54" t="s">
+      <c r="F7" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="G7" s="64">
+      <c r="G7" s="41">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H7" s="65"/>
-      <c r="I7" s="73">
+      <c r="H7" s="42"/>
+      <c r="I7" s="50">
         <v>41614</v>
       </c>
-      <c r="J7" s="76" t="s">
+      <c r="J7" s="53" t="s">
         <v>3596</v>
       </c>
-      <c r="K7" s="76" t="s">
+      <c r="K7" s="53" t="s">
         <v>3631</v>
       </c>
-      <c r="L7" s="76" t="s">
+      <c r="L7" s="53" t="s">
         <v>3632</v>
       </c>
-      <c r="M7" s="69" t="s">
+      <c r="M7" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="O7" s="70" t="s">
+      <c r="O7" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="P7" s="70" t="s">
+      <c r="P7" s="47" t="s">
         <v>3629</v>
       </c>
-      <c r="Q7" s="70" t="s">
+      <c r="Q7" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="R7" s="70">
+      <c r="R7" s="47">
         <v>145</v>
       </c>
-      <c r="S7" s="70" t="s">
+      <c r="S7" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="T7" s="71" t="s">
+      <c r="T7" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="Z7" s="55" t="s">
+      <c r="Z7" s="32" t="s">
         <v>3558</v>
       </c>
-      <c r="AA7" s="55" t="s">
+      <c r="AA7" s="32" t="s">
         <v>3559</v>
       </c>
-      <c r="AB7" s="57" t="s">
+      <c r="AB7" s="34" t="s">
         <v>3540</v>
       </c>
-      <c r="AC7" s="59">
+      <c r="AC7" s="36">
         <v>220.5</v>
       </c>
-      <c r="AD7" s="59">
+      <c r="AD7" s="36">
         <v>34.700000000000003</v>
       </c>
-      <c r="AE7" s="59" t="s">
+      <c r="AE7" s="36" t="s">
         <v>3626</v>
       </c>
-      <c r="AF7" s="59">
+      <c r="AF7" s="36">
         <v>-12.1</v>
       </c>
-      <c r="AG7" s="58"/>
-      <c r="AH7" s="61" t="s">
+      <c r="AG7" s="35"/>
+      <c r="AH7" s="38" t="s">
         <v>3627</v>
       </c>
-      <c r="AI7" s="63">
+      <c r="AI7" s="40">
         <v>4.5</v>
       </c>
-      <c r="AJ7" s="62"/>
-      <c r="AK7" s="62"/>
-      <c r="AL7" s="68">
+      <c r="AJ7" s="39"/>
+      <c r="AK7" s="39"/>
+      <c r="AL7" s="45">
         <v>45</v>
       </c>
-      <c r="AM7" s="68" t="s">
+      <c r="AM7" s="45" t="s">
         <v>3547</v>
       </c>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="28" t="s">
         <v>3601</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="29" t="s">
         <v>3619</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="30" t="s">
         <v>3621</v>
       </c>
-      <c r="D8" s="53" t="s">
+      <c r="D8" s="30" t="s">
         <v>1342</v>
       </c>
-      <c r="E8" s="54">
+      <c r="E8" s="31">
         <v>162.9</v>
       </c>
-      <c r="F8" s="54" t="s">
+      <c r="F8" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="G8" s="64">
+      <c r="G8" s="41">
         <v>10.3</v>
       </c>
-      <c r="H8" s="65"/>
-      <c r="I8" s="73">
+      <c r="H8" s="42"/>
+      <c r="I8" s="50">
         <v>41614</v>
       </c>
-      <c r="J8" s="76" t="s">
+      <c r="J8" s="53" t="s">
         <v>3596</v>
       </c>
-      <c r="K8" s="76" t="s">
+      <c r="K8" s="53" t="s">
         <v>3631</v>
       </c>
-      <c r="L8" s="76" t="s">
+      <c r="L8" s="53" t="s">
         <v>3632</v>
       </c>
-      <c r="M8" s="69" t="s">
+      <c r="M8" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="O8" s="70" t="s">
+      <c r="O8" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="P8" s="70" t="s">
+      <c r="P8" s="47" t="s">
         <v>3629</v>
       </c>
-      <c r="Q8" s="70" t="s">
+      <c r="Q8" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="R8" s="70">
+      <c r="R8" s="47">
         <v>145</v>
       </c>
-      <c r="S8" s="70" t="s">
+      <c r="S8" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="T8" s="71" t="s">
+      <c r="T8" s="48" t="s">
         <v>3571</v>
       </c>
-      <c r="Z8" s="55" t="s">
+      <c r="Z8" s="32" t="s">
         <v>3559</v>
       </c>
-      <c r="AA8" s="55" t="s">
+      <c r="AA8" s="32" t="s">
         <v>3559</v>
       </c>
-      <c r="AB8" s="57" t="s">
+      <c r="AB8" s="34" t="s">
         <v>3540</v>
       </c>
-      <c r="AC8" s="58"/>
-      <c r="AD8" s="58"/>
-      <c r="AE8" s="58"/>
-      <c r="AF8" s="58"/>
-      <c r="AG8" s="58"/>
-      <c r="AH8" s="61" t="s">
+      <c r="AC8" s="35"/>
+      <c r="AD8" s="35"/>
+      <c r="AE8" s="35"/>
+      <c r="AF8" s="35"/>
+      <c r="AG8" s="35"/>
+      <c r="AH8" s="38" t="s">
         <v>3628</v>
       </c>
-      <c r="AI8" s="63">
+      <c r="AI8" s="40">
         <v>4.5</v>
       </c>
-      <c r="AJ8" s="62"/>
-      <c r="AK8" s="62"/>
-      <c r="AL8" s="68">
+      <c r="AJ8" s="39"/>
+      <c r="AK8" s="39"/>
+      <c r="AL8" s="45">
         <v>43</v>
       </c>
-      <c r="AM8" s="68" t="s">
+      <c r="AM8" s="45" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="28" t="s">
         <v>3605</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="29" t="s">
         <v>3617</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="30" t="s">
         <v>3623</v>
       </c>
-      <c r="D9" s="53" t="s">
+      <c r="D9" s="30" t="s">
         <v>1109</v>
       </c>
-      <c r="E9" s="54">
+      <c r="E9" s="31">
         <v>132</v>
       </c>
-      <c r="F9" s="54" t="s">
+      <c r="F9" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="G9" s="64">
+      <c r="G9" s="41">
         <v>12.9</v>
       </c>
-      <c r="H9" s="66">
+      <c r="H9" s="43">
         <v>80</v>
       </c>
-      <c r="I9" s="73">
+      <c r="I9" s="50">
         <v>41614</v>
       </c>
-      <c r="J9" s="77" t="s">
+      <c r="J9" s="54" t="s">
         <v>3596</v>
       </c>
-      <c r="K9" s="77" t="s">
+      <c r="K9" s="54" t="s">
         <v>3632</v>
       </c>
-      <c r="L9" s="77" t="s">
+      <c r="L9" s="54" t="s">
         <v>3633</v>
       </c>
-      <c r="M9" s="69" t="s">
+      <c r="M9" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="O9" s="70" t="s">
+      <c r="O9" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="P9" s="70" t="s">
+      <c r="P9" s="47" t="s">
         <v>3629</v>
       </c>
-      <c r="Q9" s="70" t="s">
+      <c r="Q9" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="R9" s="70">
+      <c r="R9" s="47">
         <v>160</v>
       </c>
-      <c r="S9" s="70" t="s">
+      <c r="S9" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="T9" s="71" t="s">
+      <c r="T9" s="48" t="s">
         <v>3630</v>
       </c>
-      <c r="Z9" s="55" t="s">
+      <c r="Z9" s="32" t="s">
         <v>3558</v>
       </c>
-      <c r="AA9" s="55" t="s">
+      <c r="AA9" s="32" t="s">
         <v>3559</v>
       </c>
-      <c r="AB9" s="57" t="s">
+      <c r="AB9" s="34" t="s">
         <v>3540</v>
       </c>
-      <c r="AC9" s="59">
+      <c r="AC9" s="36">
         <v>177</v>
       </c>
-      <c r="AD9" s="59">
+      <c r="AD9" s="36">
         <v>44</v>
       </c>
-      <c r="AE9" s="59">
+      <c r="AE9" s="36">
         <v>47</v>
       </c>
-      <c r="AF9" s="59">
+      <c r="AF9" s="36">
         <v>-3.9</v>
       </c>
-      <c r="AG9" s="58"/>
-      <c r="AH9" s="60"/>
-      <c r="AI9" s="63">
+      <c r="AG9" s="35"/>
+      <c r="AH9" s="37"/>
+      <c r="AI9" s="40">
         <v>4.5</v>
       </c>
-      <c r="AJ9" s="62"/>
-      <c r="AK9" s="62"/>
-      <c r="AL9" s="68">
+      <c r="AJ9" s="39"/>
+      <c r="AK9" s="39"/>
+      <c r="AL9" s="45">
         <v>70</v>
       </c>
-      <c r="AM9" s="68" t="s">
+      <c r="AM9" s="45" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="28" t="s">
         <v>3606</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="29" t="s">
         <v>3620</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="30" t="s">
         <v>3621</v>
       </c>
-      <c r="D10" s="53" t="s">
+      <c r="D10" s="30" t="s">
         <v>1342</v>
       </c>
-      <c r="E10" s="54">
+      <c r="E10" s="31">
         <v>169</v>
       </c>
-      <c r="F10" s="54" t="s">
+      <c r="F10" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="G10" s="64">
+      <c r="G10" s="41">
         <v>11.8</v>
       </c>
-      <c r="H10" s="65"/>
-      <c r="I10" s="73">
+      <c r="H10" s="42"/>
+      <c r="I10" s="50">
         <v>41614</v>
       </c>
-      <c r="J10" s="76" t="s">
+      <c r="J10" s="53" t="s">
         <v>3596</v>
       </c>
-      <c r="K10" s="76" t="s">
+      <c r="K10" s="53" t="s">
         <v>3631</v>
       </c>
-      <c r="L10" s="76" t="s">
+      <c r="L10" s="53" t="s">
         <v>3632</v>
       </c>
-      <c r="M10" s="69" t="s">
+      <c r="M10" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="O10" s="70" t="s">
+      <c r="O10" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="P10" s="70" t="s">
+      <c r="P10" s="47" t="s">
         <v>3629</v>
       </c>
-      <c r="Q10" s="70" t="s">
+      <c r="Q10" s="47" t="s">
         <v>3530</v>
       </c>
-      <c r="R10" s="70">
+      <c r="R10" s="47">
         <v>180</v>
       </c>
-      <c r="S10" s="70" t="s">
+      <c r="S10" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="T10" s="71" t="s">
+      <c r="T10" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="Z10" s="55" t="s">
+      <c r="Z10" s="32" t="s">
         <v>3559</v>
       </c>
-      <c r="AA10" s="55" t="s">
+      <c r="AA10" s="32" t="s">
         <v>3559</v>
       </c>
-      <c r="AB10" s="56"/>
-      <c r="AC10" s="58"/>
-      <c r="AD10" s="58"/>
-      <c r="AE10" s="58"/>
-      <c r="AF10" s="58"/>
-      <c r="AG10" s="58"/>
-      <c r="AH10" s="60"/>
-      <c r="AI10" s="63">
+      <c r="AB10" s="33"/>
+      <c r="AC10" s="35"/>
+      <c r="AD10" s="35"/>
+      <c r="AE10" s="35"/>
+      <c r="AF10" s="35"/>
+      <c r="AG10" s="35"/>
+      <c r="AH10" s="37"/>
+      <c r="AI10" s="40">
         <v>4.5</v>
       </c>
-      <c r="AJ10" s="62"/>
-      <c r="AK10" s="62"/>
-      <c r="AL10" s="68">
+      <c r="AJ10" s="39"/>
+      <c r="AK10" s="39"/>
+      <c r="AL10" s="45">
         <v>48</v>
       </c>
-      <c r="AM10" s="68" t="s">
+      <c r="AM10" s="45" t="s">
         <v>138</v>
       </c>
     </row>
@@ -15345,6 +15349,20 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0" insertHyperlinks="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="30">
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="AX1:AZ1"/>
     <mergeCell ref="AT1:AW1"/>
     <mergeCell ref="A1:A2"/>
@@ -15361,20 +15379,6 @@
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="U1:U2"/>
   </mergeCells>
   <dataValidations xWindow="1791" yWindow="233" count="37">
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Example" prompt="345" sqref="AT1:AT1048576"/>
@@ -15461,7 +15465,7 @@
   <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -15483,27 +15487,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="77" t="s">
         <v>3565</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="75" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33" t="s">
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75" t="s">
         <v>126</v>
       </c>
-      <c r="I1" s="33"/>
-      <c r="J1" s="34" t="s">
+      <c r="I1" s="75"/>
+      <c r="J1" s="76" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
+      <c r="A2" s="78"/>
       <c r="B2" s="4" t="s">
         <v>119</v>
       </c>
@@ -15528,37 +15532,37 @@
       <c r="I2" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="J2" s="34"/>
+      <c r="J2" s="76"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="55" t="s">
         <v>3615</v>
       </c>
-      <c r="B3" s="78">
+      <c r="B3" s="55">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C3" s="78">
+      <c r="C3" s="55">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D3" s="78">
+      <c r="D3" s="55">
         <v>3.3</v>
       </c>
-      <c r="E3" s="78">
+      <c r="E3" s="55">
         <v>4.4000000000000004</v>
       </c>
-      <c r="F3" s="78">
+      <c r="F3" s="55">
         <v>5.5</v>
       </c>
-      <c r="G3" s="78">
+      <c r="G3" s="55">
         <v>6.6</v>
       </c>
-      <c r="H3" s="78">
+      <c r="H3" s="55">
         <v>7.7</v>
       </c>
-      <c r="I3" s="78">
+      <c r="I3" s="55">
         <v>8.8000000000000007</v>
       </c>
-      <c r="J3" s="78" t="s">
+      <c r="J3" s="55" t="s">
         <v>3634</v>
       </c>
     </row>
@@ -30972,4 +30976,24 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3635</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>